<commit_message>
adicionando versão atualizada Backlog
</commit_message>
<xml_diff>
--- a/TotemHub - Backlog.xlsx
+++ b/TotemHub - Backlog.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor.herculano\OneDrive - Accenture\Documents\Bandtec\SegundoSemestre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bandtec_TotemHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7030D6F7-1B04-4901-9BF8-3449D30A236D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E1342D-1320-4E2C-8248-42982AE59C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$B$4:$I$4</definedName>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="103">
   <si>
     <t>Nome da tarefa</t>
   </si>
@@ -257,6 +259,81 @@
   </si>
   <si>
     <t>Divisão do conteúdo da Apresentação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REQUISITOS </t>
+  </si>
+  <si>
+    <t>CLASSIFICAÇÃO</t>
+  </si>
+  <si>
+    <t>DIFICULDADE</t>
+  </si>
+  <si>
+    <t>ORDEM DE EXECUÇÃO</t>
+  </si>
+  <si>
+    <t>Utilização da ferramenta de planejamento</t>
+  </si>
+  <si>
+    <t>Definição da Regra de Negócios</t>
+  </si>
+  <si>
+    <t>Desenvolvimento do DER</t>
+  </si>
+  <si>
+    <t>Versão 1 Site Estático</t>
+  </si>
+  <si>
+    <t>Configuração do ambiente Azure</t>
+  </si>
+  <si>
+    <t>Desenvolvimento LeanUX</t>
+  </si>
+  <si>
+    <t>Definição UserStories e StoryBoard</t>
+  </si>
+  <si>
+    <t>Ideação de inovação do projeto</t>
+  </si>
+  <si>
+    <t>Definição da Proto-Persona</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da documentação do projeto</t>
+  </si>
+  <si>
+    <t>Consulta constante com especialistas</t>
+  </si>
+  <si>
+    <t>Visita para entendimento real do serviço a ser inovado</t>
+  </si>
+  <si>
+    <t>Elaboração da apresentação</t>
+  </si>
+  <si>
+    <t>Abordagem Scrum do projeto</t>
+  </si>
+  <si>
+    <t>Padronização de todos os elementos utilizados no processo</t>
+  </si>
+  <si>
+    <t>Utilização de Java para cadastro e login</t>
+  </si>
+  <si>
+    <t>Definição do projeto</t>
+  </si>
+  <si>
+    <t>Configuração do repositório Git</t>
+  </si>
+  <si>
+    <t>Definição do Backlog</t>
+  </si>
+  <si>
+    <t>Desenvolvimento do protótipo de telas</t>
+  </si>
+  <si>
+    <t>Criação do Plano de Resposta</t>
   </si>
 </sst>
 </file>
@@ -309,7 +386,7 @@
       <name val="Aharoni"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +426,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -479,21 +574,105 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2DCDB"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2DCDB"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDE9D9"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDE9D9"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2DCDB"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2DCDB"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -504,6 +683,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9ED0A3B3-F4F2-4B32-B50E-A37B122A0B35}" name="Tabela1" displayName="Tabela1" ref="D2:G23" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
+  <autoFilter ref="D2:G23" xr:uid="{9ED0A3B3-F4F2-4B32-B50E-A37B122A0B35}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:G23">
+    <sortCondition ref="G2:G23"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A78A8EBC-A65E-494E-8622-E8B79E58F16B}" name="REQUISITOS " dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{F112FCB8-83DA-4826-91D8-90CB36F51B3E}" name="CLASSIFICAÇÃO" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{E1A2DDB5-778D-4ECE-9E05-32946A104EAC}" name="DIFICULDADE" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{A6EEEE49-7FB7-4FCE-AC8A-E8E59952F4B5}" name="ORDEM DE EXECUÇÃO" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -830,45 +1025,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.75" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.9140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.58203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" ht="30.5" x14ac:dyDescent="0.65">
-      <c r="B2" s="28" t="s">
+    <row r="1" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:14" ht="30.75" x14ac:dyDescent="0.45">
+      <c r="B2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
       <c r="N2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="7" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
@@ -897,7 +1092,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>47</v>
       </c>
@@ -923,7 +1118,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="25" t="s">
         <v>47</v>
       </c>
@@ -949,7 +1144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
         <v>47</v>
       </c>
@@ -975,7 +1170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="25" t="s">
         <v>47</v>
       </c>
@@ -1001,7 +1196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="27" t="s">
         <v>47</v>
       </c>
@@ -1027,7 +1222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="26" t="s">
         <v>47</v>
       </c>
@@ -1053,7 +1248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
         <v>47</v>
       </c>
@@ -1079,7 +1274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
         <v>47</v>
       </c>
@@ -1105,7 +1300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>47</v>
       </c>
@@ -1131,7 +1326,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="25" t="s">
         <v>47</v>
       </c>
@@ -1157,7 +1352,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="25" t="s">
         <v>47</v>
       </c>
@@ -1183,8 +1378,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="30"/>
+    <row r="16" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="28"/>
       <c r="B16" s="9" t="s">
         <v>47</v>
       </c>
@@ -1210,8 +1405,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="30"/>
+    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
       <c r="B17" s="26" t="s">
         <v>47</v>
       </c>
@@ -1237,8 +1432,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="30"/>
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
       <c r="B18" s="26" t="s">
         <v>47</v>
       </c>
@@ -1264,8 +1459,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="30"/>
+    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
       <c r="B19" s="26" t="s">
         <v>47</v>
       </c>
@@ -1291,8 +1486,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="30"/>
+    <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28"/>
       <c r="B20" s="9" t="s">
         <v>47</v>
       </c>
@@ -1318,8 +1513,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="30"/>
+    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
       <c r="B21" s="26" t="s">
         <v>47</v>
       </c>
@@ -1345,8 +1540,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="30"/>
+    <row r="22" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
       <c r="B22" s="26" t="s">
         <v>47</v>
       </c>
@@ -1372,8 +1567,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="30"/>
+    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
       <c r="B23" s="25" t="s">
         <v>47</v>
       </c>
@@ -1399,8 +1594,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="30"/>
+    <row r="24" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="28"/>
       <c r="B24" s="14" t="s">
         <v>47</v>
       </c>
@@ -1426,9 +1621,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31" t="s">
+    <row r="25" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="22" t="s">
@@ -1453,9 +1648,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="30"/>
-      <c r="B26" s="31" t="s">
+    <row r="26" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="28"/>
+      <c r="B26" s="29" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="22" t="s">
@@ -1480,8 +1675,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="30"/>
+    <row r="27" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="28"/>
       <c r="B27" s="26" t="s">
         <v>47</v>
       </c>
@@ -1507,8 +1702,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="30"/>
+    <row r="28" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
       <c r="B28" s="14" t="s">
         <v>47</v>
       </c>
@@ -1534,8 +1729,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="30"/>
+    <row r="29" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="28"/>
       <c r="B29" s="26" t="s">
         <v>47</v>
       </c>
@@ -1561,8 +1756,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="30"/>
+    <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="28"/>
       <c r="B30" s="9" t="s">
         <v>47</v>
       </c>
@@ -1588,8 +1783,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="30"/>
+    <row r="31" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="28"/>
       <c r="B31" s="25" t="s">
         <v>47</v>
       </c>
@@ -1615,7 +1810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="25" t="s">
         <v>47</v>
       </c>
@@ -1641,7 +1836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="25" t="s">
         <v>47</v>
       </c>
@@ -1667,7 +1862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="25" t="s">
         <v>47</v>
       </c>
@@ -1693,7 +1888,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="25" t="s">
         <v>47</v>
       </c>
@@ -1719,7 +1914,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="25" t="s">
         <v>72</v>
       </c>
@@ -1745,7 +1940,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="25" t="s">
         <v>72</v>
       </c>
@@ -1771,7 +1966,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="9" t="s">
         <v>47</v>
       </c>
@@ -1797,7 +1992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="25" t="s">
         <v>47</v>
       </c>
@@ -1823,7 +2018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="14" t="s">
         <v>47</v>
       </c>
@@ -1849,7 +2044,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="26" t="s">
         <v>47</v>
       </c>
@@ -1875,7 +2070,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="26" t="s">
         <v>72</v>
       </c>
@@ -1901,7 +2096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="26" t="s">
         <v>47</v>
       </c>
@@ -1927,7 +2122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
         <v>72</v>
       </c>
@@ -1953,7 +2148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="25" t="s">
         <v>72</v>
       </c>
@@ -1979,7 +2174,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="25" t="s">
         <v>72</v>
       </c>
@@ -2005,7 +2200,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
         <v>47</v>
       </c>
@@ -2031,7 +2226,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="25" t="s">
         <v>47</v>
       </c>
@@ -2057,7 +2252,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="25" t="s">
         <v>47</v>
       </c>
@@ -2083,7 +2278,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="14" t="s">
         <v>72</v>
       </c>
@@ -2109,7 +2304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="9" t="s">
         <v>72</v>
       </c>
@@ -2135,7 +2330,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="25" t="s">
         <v>72</v>
       </c>
@@ -2161,7 +2356,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="9" t="s">
         <v>47</v>
       </c>
@@ -2187,7 +2382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="25" t="s">
         <v>47</v>
       </c>
@@ -2213,7 +2408,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="25" t="s">
         <v>47</v>
       </c>
@@ -2239,7 +2434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="25" t="s">
         <v>47</v>
       </c>
@@ -2281,4 +2476,381 @@
     <ignoredError sqref="C50 D3:F3 G3:I3 D5 E50 C3:C5 H9:I9 C9:D9 H13:I13 C13:D13 H16:I16 C16 I20 C20:E20 G24:I24 C24:D24 H28:I28 C28 H30:I30 C30 I38 C38 H40:I40 C40 H44:I44 D44 I47 H5:I5 G4:H4 D4:E4 I50" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED08078-4B5B-4569-8B77-E92900F2E0BD}">
+  <dimension ref="D2:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="48.5" style="32" customWidth="1"/>
+    <col min="5" max="5" width="21.5" style="32" customWidth="1"/>
+    <col min="6" max="6" width="21.375" style="32" customWidth="1"/>
+    <col min="7" max="7" width="23.75" style="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="33">
+        <v>3</v>
+      </c>
+      <c r="G3" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="33">
+        <v>3</v>
+      </c>
+      <c r="G4" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="33">
+        <v>3</v>
+      </c>
+      <c r="G5" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="33">
+        <v>14</v>
+      </c>
+      <c r="G6" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="33">
+        <v>8</v>
+      </c>
+      <c r="G7" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="33">
+        <v>5</v>
+      </c>
+      <c r="G8" s="33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="33">
+        <v>8</v>
+      </c>
+      <c r="G9" s="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="33">
+        <v>8</v>
+      </c>
+      <c r="G10" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="33">
+        <v>8</v>
+      </c>
+      <c r="G11" s="33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="33">
+        <v>8</v>
+      </c>
+      <c r="G12" s="33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="35">
+        <v>8</v>
+      </c>
+      <c r="G13" s="35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="35">
+        <v>5</v>
+      </c>
+      <c r="G14" s="35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="35">
+        <v>3</v>
+      </c>
+      <c r="G15" s="35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="33">
+        <v>21</v>
+      </c>
+      <c r="G16" s="33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="35">
+        <v>5</v>
+      </c>
+      <c r="G17" s="35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="33">
+        <v>14</v>
+      </c>
+      <c r="G18" s="33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="33">
+        <v>14</v>
+      </c>
+      <c r="G19" s="33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D20" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="35">
+        <v>8</v>
+      </c>
+      <c r="G20" s="35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D21" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="33">
+        <v>14</v>
+      </c>
+      <c r="G21" s="33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D22" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="33">
+        <v>3</v>
+      </c>
+      <c r="G22" s="33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="34">
+        <v>3</v>
+      </c>
+      <c r="G23" s="34">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C4F468C4-E136-476B-90C2-BBA699E6D5C3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C4F468C4-E136-476B-90C2-BBA699E6D5C3}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746770E9-57AE-43AC-96BA-C5185126D1A5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
subindo versão final Backlog
</commit_message>
<xml_diff>
--- a/TotemHub - Backlog.xlsx
+++ b/TotemHub - Backlog.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor.herculano\OneDrive - Accenture\Documents\Bandtec\SegundoSemestre\Bandtec_TotemHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bandtec_TotemHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FC363B-60F9-4A7D-8B05-C2CEC3D3E446}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670036AE-2118-4EBD-8F20-39B1752DC284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de reqs." sheetId="3" r:id="rId1"/>
     <sheet name="Refatoração Estrutura" sheetId="4" r:id="rId2"/>
+    <sheet name="User Story" sheetId="5" r:id="rId3"/>
+    <sheet name="Planilha2" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Lista de reqs.'!$G$4:$I$4</definedName>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="63">
   <si>
     <t>Essencial</t>
   </si>
@@ -119,17 +121,107 @@
     <t>Sistema de recompensas</t>
   </si>
   <si>
-    <t>Backlog - TotemHub (Refatoração)</t>
-  </si>
-  <si>
     <t>Backlog - TotemHub (As Is)</t>
+  </si>
+  <si>
+    <t>Parte de Entrar em Contato</t>
+  </si>
+  <si>
+    <t>Design Intuitivo / Padronizado</t>
+  </si>
+  <si>
+    <t>Sistema de recompensas para usuário</t>
+  </si>
+  <si>
+    <t>UX#001</t>
+  </si>
+  <si>
+    <t>UX#004</t>
+  </si>
+  <si>
+    <t>UX#005</t>
+  </si>
+  <si>
+    <t>UX#002</t>
+  </si>
+  <si>
+    <t>UX#003</t>
+  </si>
+  <si>
+    <t>UX#003 (teste)</t>
+  </si>
+  <si>
+    <t>Inovação</t>
+  </si>
+  <si>
+    <t>Backlog - TotemHub</t>
+  </si>
+  <si>
+    <t>Site institucional para navegação do usuário</t>
+  </si>
+  <si>
+    <t>Protótipo para homologação da idéia com o cliente</t>
+  </si>
+  <si>
+    <t>Cadastro e login de usuários do site</t>
+  </si>
+  <si>
+    <t>HomePage para navegação pelo site</t>
+  </si>
+  <si>
+    <t>Service Desk para conexão do cliente com o suporte</t>
+  </si>
+  <si>
+    <t>Página de Sobre para aproximação do cliente com a soluçao</t>
+  </si>
+  <si>
+    <t>Parte de Contato para acesso de leads com os fornecedores da aplicação</t>
+  </si>
+  <si>
+    <t>API de consulta e cadastro para navegação e gerenciamento do site</t>
+  </si>
+  <si>
+    <t>Monitoramento de Sistemas Operacionais de totens para visualização e tomada de decisões</t>
+  </si>
+  <si>
+    <t>Cadastro de MultiUsuários relacionados a mesma estação para gerenciamento pelo próprio responsável da estação</t>
+  </si>
+  <si>
+    <t>Dashboard dinâmicas</t>
+  </si>
+  <si>
+    <t>Funcionamento da dashboard de acordo com dados captados do SO</t>
+  </si>
+  <si>
+    <t>Indicadores informando monitor sobre o funcionamento do totem</t>
+  </si>
+  <si>
+    <t>Responsividade para funcionamento orgânico do site (melhor adaptação)</t>
+  </si>
+  <si>
+    <t>Ambiente Linux captando dados de funcionamento da CPU</t>
+  </si>
+  <si>
+    <t>Desgin intuitivo para navegação fluída do site</t>
+  </si>
+  <si>
+    <t>Controle de permissão para segurança do site</t>
+  </si>
+  <si>
+    <t>Dashboard Intuitiva</t>
+  </si>
+  <si>
+    <t>Dashboard intuitiva para melhor gerenciamento do monitor</t>
+  </si>
+  <si>
+    <t>Forma de atrair o público e diferenciar a aplicação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -166,8 +258,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +321,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF97"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -461,17 +566,6 @@
     </border>
     <border>
       <left style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -481,19 +575,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </right>
-      <top style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -556,21 +637,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -598,109 +667,177 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color theme="3" tint="-0.249977111117893"/>
         </left>
@@ -709,55 +846,55 @@
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="3" tint="-0.249977111117893"/>
+        </left>
         <right style="medium">
           <color theme="3" tint="-0.249977111117893"/>
         </right>
-        <vertical/>
+        <top/>
+        <bottom style="medium">
+          <color theme="3" tint="-0.249977111117893"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <right style="medium">
+          <color theme="3" tint="-0.249977111117893"/>
+        </right>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF97"/>
+      <color rgb="FFF6F648"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -769,15 +906,131 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6CA24F5-7B9E-4095-81A3-2C653F8E19B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1619250" y="714375"/>
+          <a:ext cx="7639050" cy="4067175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9012F7D0-F304-469E-AAD7-77FEDC3F1EAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2105025" y="66675"/>
+          <a:ext cx="5343525" cy="4067175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AD0C298-A3C4-4B6D-A826-3F4FDA3611BC}" name="Tabela2" displayName="Tabela2" ref="C4:H14" totalsRowShown="0" headerRowDxfId="3" dataDxfId="7">
-  <autoFilter ref="C4:H14" xr:uid="{E4E6A3FB-FD8D-435E-AFC5-2349C9D21F73}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{97D85B41-9860-4CD6-B68A-0F415CA5CC92}" name="Estado" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{53156FB0-92E5-4B86-BE2B-46C7F61C34DC}" name="Artefato de referência" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AD0C298-A3C4-4B6D-A826-3F4FDA3611BC}" name="Tabela2" displayName="Tabela2" ref="C4:I22" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="C4:I22" xr:uid="{E4E6A3FB-FD8D-435E-AFC5-2349C9D21F73}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{97D85B41-9860-4CD6-B68A-0F415CA5CC92}" name="Estado" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{53156FB0-92E5-4B86-BE2B-46C7F61C34DC}" name="Artefato de referência" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{FB97AF01-D5F2-4F8A-86F7-BCD92C00AE2F}" name="Requisito" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{AB0A7A6A-87D8-4F19-BC58-69B293139831}" name="Descrição do requisito" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{0A12B184-8A4D-426F-9E70-E9503B1100F2}" name="Essencial" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B79ECEB9-B207-4E45-873B-790E6DCAEC3A}" name="Importante" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B79ECEB9-B207-4E45-873B-790E6DCAEC3A}" name="Importante" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{B0EE7D0E-8FE0-42D4-83DE-B48C430B7A72}" name="Desejavel" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1108,275 +1361,275 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746770E9-57AE-43AC-96BA-C5185126D1A5}">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD39"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="8.6640625" style="51"/>
-    <col min="7" max="7" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="8.6640625" style="51"/>
-    <col min="16" max="16384" width="8.6640625" style="2"/>
+    <col min="1" max="6" width="8.625" style="18"/>
+    <col min="7" max="7" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="8.625" style="18"/>
+    <col min="16" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:23" s="51" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="7:23" ht="31" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="G2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="W2" s="6" t="s">
+    <row r="1" spans="7:23" s="18" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="7:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
+      <c r="W2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="7:23" s="51" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I3" s="52"/>
-      <c r="W3" s="53" t="s">
+    <row r="3" spans="7:23" s="18" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="19"/>
+      <c r="W3" s="20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="7:23" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="7" t="s">
+    <row r="4" spans="7:23" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="W4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G5" s="9" t="s">
+    <row r="5" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G6" s="11" t="s">
+    <row r="6" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G7" s="11" t="s">
+    <row r="7" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="W7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G8" s="11" t="s">
+    <row r="8" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W8" s="6" t="s">
+      <c r="W8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G9" s="11" t="s">
+    <row r="9" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="W9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G10" s="11" t="s">
+    <row r="10" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G11" s="11" t="s">
+    <row r="11" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G12" s="11" t="s">
+    <row r="12" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G13" s="11" t="s">
+    <row r="13" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G14" s="11" t="s">
+    <row r="14" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G15" s="11" t="s">
+    <row r="15" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="7:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G16" s="11" t="s">
+    <row r="16" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="7:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G17" s="11" t="s">
+    <row r="17" spans="7:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="7:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G18" s="9" t="s">
+    <row r="18" spans="7:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="7:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G19" s="16" t="s">
+    <row r="19" spans="7:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="7:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G20" s="16" t="s">
+    <row r="20" spans="7:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="7:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G21" s="16" t="s">
+    <row r="21" spans="7:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="7:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G22" s="18" t="s">
+    <row r="22" spans="7:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="7:9" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="33" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="34" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="37" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="38" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="39" s="51" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="7:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="G4:I4" xr:uid="{335B71D8-2091-432D-8DE4-15DDF27DD779}"/>
   <mergeCells count="1">
@@ -1396,329 +1649,538 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D365EA23-5304-45D0-B9B5-2768DD50B9BF}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.6640625" style="46"/>
-    <col min="3" max="3" width="13.58203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.08203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.58203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
-    <col min="9" max="17" width="8.6640625" style="46"/>
+    <col min="1" max="2" width="8.625" style="15"/>
+    <col min="3" max="3" width="13.625" style="57" customWidth="1"/>
+    <col min="4" max="4" width="24.125" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.125" style="57" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.25" style="57" customWidth="1"/>
+    <col min="7" max="7" width="13.625" style="57" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="57" customWidth="1"/>
+    <col min="9" max="9" width="13.375" style="57" customWidth="1"/>
+    <col min="10" max="18" width="8.625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-    </row>
-    <row r="2" spans="2:8" s="46" customFormat="1" ht="31" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="C2" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-    </row>
-    <row r="3" spans="2:8" s="46" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="47"/>
-      <c r="C4" s="21" t="s">
+    <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="2:9" s="15" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="2:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="16"/>
+      <c r="C4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="H4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="I4" s="27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="47"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="44"/>
-    </row>
-    <row r="6" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="47"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="45"/>
-    </row>
-    <row r="7" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="48"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="43"/>
-    </row>
-    <row r="8" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="47"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="41"/>
-    </row>
-    <row r="9" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="47"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="43"/>
-    </row>
-    <row r="10" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="47"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="47"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="43"/>
-    </row>
-    <row r="12" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="47"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="41"/>
-    </row>
-    <row r="13" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="47"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="42"/>
-    </row>
-    <row r="14" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="47"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="2:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-    </row>
-    <row r="16" spans="2:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-    </row>
-    <row r="17" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-    </row>
-    <row r="18" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-    </row>
-    <row r="19" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-    </row>
-    <row r="20" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-    </row>
-    <row r="21" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-    </row>
-    <row r="22" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-    </row>
-    <row r="23" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-    </row>
-    <row r="24" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-    </row>
-    <row r="25" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-    </row>
-    <row r="26" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-    </row>
-    <row r="27" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-    </row>
-    <row r="28" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-    </row>
-    <row r="29" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-    </row>
-    <row r="30" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-    </row>
-    <row r="31" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-    </row>
-    <row r="32" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-    </row>
-    <row r="33" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-    </row>
-    <row r="34" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="49"/>
-    </row>
-    <row r="35" spans="3:8" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
+    <row r="5" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="16"/>
+      <c r="C5" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="33"/>
+    </row>
+    <row r="6" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="16"/>
+      <c r="C6" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="37"/>
+    </row>
+    <row r="7" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="17"/>
+      <c r="C7" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="31"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="16"/>
+      <c r="C8" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="31"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="41"/>
+    </row>
+    <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16"/>
+      <c r="C9" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39"/>
+    </row>
+    <row r="10" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16"/>
+      <c r="C10" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="31"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="41"/>
+    </row>
+    <row r="11" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16"/>
+      <c r="C11" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="39"/>
+    </row>
+    <row r="12" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="16"/>
+      <c r="C12" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="31"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="41"/>
+    </row>
+    <row r="13" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="16"/>
+      <c r="C13" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="31"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="47"/>
+    </row>
+    <row r="14" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="16"/>
+      <c r="C14" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="31"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="52"/>
+    </row>
+    <row r="15" spans="2:9" s="24" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="60"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="61"/>
+    </row>
+    <row r="16" spans="2:9" s="24" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="60"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="64"/>
+    </row>
+    <row r="17" spans="3:9" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="3:9" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="31"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="41"/>
+    </row>
+    <row r="19" spans="3:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="53"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="41"/>
+    </row>
+    <row r="20" spans="3:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="53"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="41"/>
+    </row>
+    <row r="21" spans="3:9" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="53"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="41"/>
+    </row>
+    <row r="22" spans="3:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="53"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="55"/>
+    </row>
+    <row r="23" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+    </row>
+    <row r="24" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+    </row>
+    <row r="25" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+    </row>
+    <row r="26" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+    </row>
+    <row r="27" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+    </row>
+    <row r="28" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+    </row>
+    <row r="29" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+    </row>
+    <row r="30" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+    </row>
+    <row r="31" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+    </row>
+    <row r="32" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+    </row>
+    <row r="33" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+    </row>
+    <row r="34" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C2:I2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288FC3E7-48B0-4EA1-84BD-030D133D4615}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECFABF79-7CBD-4857-A8FB-1108C995F101}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>